<commit_message>
fixed regex for TH
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/test-msisdns-invalid.xlsx
+++ b/Tests/Fixtures/test-msisdns-invalid.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="test-msisdns-invalid.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -810,7 +810,7 @@
       </c>
       <c r="D2">
         <f ca="1">RANDBETWEEN(1,9)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>